<commit_message>
Task and Subtask implemented (read-only)
</commit_message>
<xml_diff>
--- a/database/dataset.xlsx
+++ b/database/dataset.xlsx
@@ -5,22 +5,22 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.leite\Fugro\AME Digital Transformation - Documents\02-Digital Solutions\TimeBuilder2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://fugro.sharepoint.com/sites/AMEDigitalTransformation/Shared Documents/02-Digital Solutions/24-99 Project Control Workbook/VS Workspace/TimeBuilderF/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEAB3D11-B5E8-4021-A263-A133CBD2DA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{DEAB3D11-B5E8-4021-A263-A133CBD2DA33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{40BFD54B-BB46-431E-B485-734B76798899}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
     <sheet name="Projects" sheetId="2" r:id="rId2"/>
     <sheet name="Tasks" sheetId="3" r:id="rId3"/>
-    <sheet name="Sub-tasks" sheetId="4" r:id="rId4"/>
+    <sheet name="Subtasks" sheetId="4" r:id="rId4"/>
     <sheet name="Task-status" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Sub-tasks'!$A$1:$B$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Subtasks!$A$1:$B$24</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
@@ -119,9 +119,6 @@
     <t>Overhead</t>
   </si>
   <si>
-    <t>Sub-task</t>
-  </si>
-  <si>
     <t>Lidar Buildings</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>On Hold</t>
+  </si>
+  <si>
+    <t>Subtask</t>
   </si>
 </sst>
 </file>
@@ -814,8 +814,8 @@
   </sheetPr>
   <dimension ref="A1:D42"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -826,7 +826,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>70</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>15</v>
@@ -842,7 +842,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
@@ -850,7 +850,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
@@ -885,7 +885,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
@@ -901,7 +901,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>16</v>
@@ -909,7 +909,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B11" t="s">
         <v>17</v>
@@ -917,7 +917,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
         <v>17</v>
@@ -925,7 +925,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
         <v>17</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
         <v>18</v>
@@ -941,7 +941,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B15" t="s">
         <v>18</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
@@ -957,7 +957,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" t="s">
         <v>18</v>
@@ -965,7 +965,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -973,7 +973,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>19</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>19</v>
@@ -997,7 +997,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B22" t="s">
         <v>19</v>
@@ -1005,7 +1005,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
         <v>19</v>
@@ -1013,7 +1013,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
         <v>19</v>
@@ -1021,7 +1021,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
         <v>20</v>
@@ -1029,7 +1029,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
         <v>20</v>
@@ -1037,7 +1037,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
         <v>20</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B28" t="s">
         <v>20</v>
@@ -1053,7 +1053,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" t="s">
         <v>20</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" t="s">
         <v>20</v>
@@ -1077,7 +1077,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B32" t="s">
         <v>21</v>
@@ -1085,7 +1085,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
         <v>21</v>
@@ -1093,7 +1093,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s">
         <v>21</v>
@@ -1125,7 +1125,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B38" t="s">
         <v>22</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B40" t="s">
         <v>22</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B41" t="s">
         <v>22</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B42" t="s">
         <v>22</v>
@@ -1172,7 +1172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F88C033-3664-47DB-955C-4A11134557AE}">
   <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1183,17 +1183,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1202,6 +1202,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a884885c-9ce3-4d9b-b5bb-db3e12494020">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0141fd56-53fa-448d-9adf-d9c8de32dc10" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100011DE5FAC43FB5448EAD2E36FE625047" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="976732a8ee3041dab3ac5d8a1e7539a2">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a884885c-9ce3-4d9b-b5bb-db3e12494020" xmlns:ns3="0141fd56-53fa-448d-9adf-d9c8de32dc10" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="67a519c47cd10f1bf67da1dd268ad3bf" ns2:_="" ns3:_="">
     <xsd:import namespace="a884885c-9ce3-4d9b-b5bb-db3e12494020"/>
@@ -1424,34 +1444,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a884885c-9ce3-4d9b-b5bb-db3e12494020">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0141fd56-53fa-448d-9adf-d9c8de32dc10" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48AA0987-B8A2-4622-92E2-5B6AAC803306}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E64C3F3-50BF-4AB8-8E93-FD64FF3B43B1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="a884885c-9ce3-4d9b-b5bb-db3e12494020"/>
+    <ds:schemaRef ds:uri="0141fd56-53fa-448d-9adf-d9c8de32dc10"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D653CB89-4D6C-4AAB-98F7-1981EE6C5015}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D653CB89-4D6C-4AAB-98F7-1981EE6C5015}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1E64C3F3-50BF-4AB8-8E93-FD64FF3B43B1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{48AA0987-B8A2-4622-92E2-5B6AAC803306}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="a884885c-9ce3-4d9b-b5bb-db3e12494020"/>
+    <ds:schemaRef ds:uri="0141fd56-53fa-448d-9adf-d9c8de32dc10"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>